<commit_message>
Modified correct coordinates for TU Delft Campus to Parking P1 (Aula).
</commit_message>
<xml_diff>
--- a/Matrices_Stations.xlsx
+++ b/Matrices_Stations.xlsx
@@ -544,7 +544,7 @@
         <v>217.32</v>
       </c>
       <c r="N2" t="n">
-        <v>70.64</v>
+        <v>72.84</v>
       </c>
     </row>
     <row r="3">
@@ -590,7 +590,7 @@
         <v>219.2</v>
       </c>
       <c r="N3" t="n">
-        <v>15.72</v>
+        <v>12.69</v>
       </c>
     </row>
     <row r="4">
@@ -636,7 +636,7 @@
         <v>245.52</v>
       </c>
       <c r="N4" t="n">
-        <v>12.62</v>
+        <v>14.83</v>
       </c>
     </row>
     <row r="5">
@@ -682,7 +682,7 @@
         <v>178.15</v>
       </c>
       <c r="N5" t="n">
-        <v>63.81</v>
+        <v>66.01000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -728,7 +728,7 @@
         <v>87.95</v>
       </c>
       <c r="N6" t="n">
-        <v>130.81</v>
+        <v>126.49</v>
       </c>
     </row>
     <row r="7">
@@ -774,7 +774,7 @@
         <v>127.82</v>
       </c>
       <c r="N7" t="n">
-        <v>98.91</v>
+        <v>94.58</v>
       </c>
     </row>
     <row r="8">
@@ -820,7 +820,7 @@
         <v>212.36</v>
       </c>
       <c r="N8" t="n">
-        <v>90.3</v>
+        <v>92.51000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -866,7 +866,7 @@
         <v>397.92</v>
       </c>
       <c r="N9" t="n">
-        <v>237.42</v>
+        <v>239.63</v>
       </c>
     </row>
     <row r="10">
@@ -912,7 +912,7 @@
         <v>148.22</v>
       </c>
       <c r="N10" t="n">
-        <v>68.98</v>
+        <v>64.65000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -958,7 +958,7 @@
         <v>139.89</v>
       </c>
       <c r="N11" t="n">
-        <v>136.03</v>
+        <v>131.73</v>
       </c>
     </row>
     <row r="12">
@@ -1004,7 +1004,7 @@
         <v>323.55</v>
       </c>
       <c r="N12" t="n">
-        <v>193.75</v>
+        <v>195.95</v>
       </c>
     </row>
     <row r="13">
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>237.48</v>
+        <v>233.15</v>
       </c>
     </row>
     <row r="14">
@@ -1060,40 +1060,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>67.01000000000001</v>
+        <v>68.13</v>
       </c>
       <c r="C14" t="n">
-        <v>15.66</v>
+        <v>12.4</v>
       </c>
       <c r="D14" t="n">
-        <v>11.63</v>
+        <v>12.66</v>
       </c>
       <c r="E14" t="n">
-        <v>65.45999999999999</v>
+        <v>65.33</v>
       </c>
       <c r="F14" t="n">
-        <v>131.5</v>
+        <v>128.24</v>
       </c>
       <c r="G14" t="n">
-        <v>99.34</v>
+        <v>96.09</v>
       </c>
       <c r="H14" t="n">
-        <v>90.55</v>
+        <v>91.66</v>
       </c>
       <c r="I14" t="n">
-        <v>238.39</v>
+        <v>239.5</v>
       </c>
       <c r="J14" t="n">
-        <v>67.39</v>
+        <v>64.13</v>
       </c>
       <c r="K14" t="n">
-        <v>134.62</v>
+        <v>131.37</v>
       </c>
       <c r="L14" t="n">
-        <v>194.58</v>
+        <v>195.69</v>
       </c>
       <c r="M14" t="n">
-        <v>236.67</v>
+        <v>233.41</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>9475.48</v>
       </c>
       <c r="N2" t="n">
-        <v>3502.66</v>
+        <v>3428.58</v>
       </c>
     </row>
     <row r="3">
@@ -1274,7 +1274,7 @@
         <v>8869.08</v>
       </c>
       <c r="N3" t="n">
-        <v>1369.74</v>
+        <v>1105.12</v>
       </c>
     </row>
     <row r="4">
@@ -1320,7 +1320,7 @@
         <v>9552.030000000001</v>
       </c>
       <c r="N4" t="n">
-        <v>1005.84</v>
+        <v>931.77</v>
       </c>
     </row>
     <row r="5">
@@ -1366,7 +1366,7 @@
         <v>7816.57</v>
       </c>
       <c r="N5" t="n">
-        <v>3193.77</v>
+        <v>3119.69</v>
       </c>
     </row>
     <row r="6">
@@ -1412,7 +1412,7 @@
         <v>4527.85</v>
       </c>
       <c r="N6" t="n">
-        <v>5970.83</v>
+        <v>6065.56</v>
       </c>
     </row>
     <row r="7">
@@ -1458,7 +1458,7 @@
         <v>5818.54</v>
       </c>
       <c r="N7" t="n">
-        <v>4504.53</v>
+        <v>4599.27</v>
       </c>
     </row>
     <row r="8">
@@ -1504,7 +1504,7 @@
         <v>9198.709999999999</v>
       </c>
       <c r="N8" t="n">
-        <v>4267.96</v>
+        <v>4193.88</v>
       </c>
     </row>
     <row r="9">
@@ -1550,7 +1550,7 @@
         <v>13319.33</v>
       </c>
       <c r="N9" t="n">
-        <v>10230.57</v>
+        <v>10156.5</v>
       </c>
     </row>
     <row r="10">
@@ -1596,7 +1596,7 @@
         <v>6761.25</v>
       </c>
       <c r="N10" t="n">
-        <v>3441.93</v>
+        <v>3536.67</v>
       </c>
     </row>
     <row r="11">
@@ -1642,7 +1642,7 @@
         <v>6539.68</v>
       </c>
       <c r="N11" t="n">
-        <v>6166.58</v>
+        <v>6262.38</v>
       </c>
     </row>
     <row r="12">
@@ -1688,7 +1688,7 @@
         <v>13945.57</v>
       </c>
       <c r="N12" t="n">
-        <v>8597.200000000001</v>
+        <v>8523.120000000001</v>
       </c>
     </row>
     <row r="13">
@@ -1734,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>9133.82</v>
+        <v>9228.549999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1744,40 +1744,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3597.8</v>
+        <v>3537.2</v>
       </c>
       <c r="C14" t="n">
-        <v>1361.5</v>
+        <v>1066.93</v>
       </c>
       <c r="D14" t="n">
-        <v>1095.17</v>
+        <v>1053.47</v>
       </c>
       <c r="E14" t="n">
-        <v>3314.07</v>
+        <v>3172.86</v>
       </c>
       <c r="F14" t="n">
-        <v>6356.72</v>
+        <v>6062.15</v>
       </c>
       <c r="G14" t="n">
-        <v>4700.08</v>
+        <v>4405.5</v>
       </c>
       <c r="H14" t="n">
-        <v>4212.99</v>
+        <v>4152.39</v>
       </c>
       <c r="I14" t="n">
-        <v>10406.96</v>
+        <v>10346.36</v>
       </c>
       <c r="J14" t="n">
-        <v>3488.09</v>
+        <v>3193.51</v>
       </c>
       <c r="K14" t="n">
-        <v>6164.39</v>
+        <v>5869.82</v>
       </c>
       <c r="L14" t="n">
-        <v>8638.18</v>
+        <v>8577.59</v>
       </c>
       <c r="M14" t="n">
-        <v>9360.32</v>
+        <v>9065.74</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>

</xml_diff>